<commit_message>
stocks: removed [manuf_date] attribute.
</commit_message>
<xml_diff>
--- a/htdocs/assets/stocks.xlsx
+++ b/htdocs/assets/stocks.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t xml:space="preserve">Название продукта</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Дата производства</t>
   </si>
   <si>
     <t xml:space="preserve">Остаток на складе</t>
@@ -383,7 +380,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -403,13 +400,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="14.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="4" width="13.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="34.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="13.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="5" width="11.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="3" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="4.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="62" min="22" style="6" width="8.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="63" style="7" width="8.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="5" width="11.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="3" width="19.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="4.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="61" min="21" style="6" width="8.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="62" style="7" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -429,10 +425,10 @@
       <c r="O1" s="10"/>
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="10"/>
-      <c r="AMI1" s="12"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="10"/>
+      <c r="AMH1" s="12"/>
+      <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -487,17 +483,14 @@
       <c r="Q2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="14" t="s">
+      <c r="R2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="S2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="T2" s="17" t="s">
         <v>19</v>
-      </c>
-      <c r="U2" s="17" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -547,22 +540,19 @@
         <v>15</v>
       </c>
       <c r="P3" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="18" t="s">
+      <c r="R3" s="19" t="n">
+        <v>19</v>
+      </c>
+      <c r="S3" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="T3" s="17" t="s">
         <v>22</v>
-      </c>
-      <c r="R3" s="16" t="n">
-        <v>18</v>
-      </c>
-      <c r="S3" s="19" t="n">
-        <v>19</v>
-      </c>
-      <c r="T3" s="18" t="n">
-        <v>20</v>
-      </c>
-      <c r="U3" s="17" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>